<commit_message>
Example data format for calibration procedure
</commit_message>
<xml_diff>
--- a/HAMMOND_Data.xlsx
+++ b/HAMMOND_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="12048" windowHeight="6336"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="12048" windowHeight="6336" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Profiles" sheetId="2" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>deg</t>
   </si>
   <si>
-    <t>not available yet!</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -321,6 +318,9 @@
   </si>
   <si>
     <t>Arthur Capet (b)</t>
+  </si>
+  <si>
+    <t>not available yet</t>
   </si>
 </sst>
 </file>
@@ -329,7 +329,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
-    <numFmt numFmtId="170" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -416,7 +416,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,22 +759,22 @@
         <v>4</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>1</v>
@@ -783,22 +783,22 @@
         <v>6</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="S1" s="5" t="s">
         <v>2</v>
@@ -807,45 +807,45 @@
         <v>7</v>
       </c>
       <c r="U1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="AE1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF1" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11">
@@ -905,7 +905,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11">
@@ -973,7 +973,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11">
@@ -1041,7 +1041,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11">
@@ -1109,7 +1109,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11">
@@ -1177,7 +1177,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11">
@@ -1245,7 +1245,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11">
@@ -1313,7 +1313,7 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11">
@@ -1381,7 +1381,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11">
@@ -1449,7 +1449,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11">
@@ -1507,7 +1507,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11">
@@ -1567,7 +1567,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11">
@@ -1635,7 +1635,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11">
@@ -1703,7 +1703,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="11">
@@ -1761,7 +1761,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11">
@@ -1829,7 +1829,7 @@
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11">
@@ -1897,7 +1897,7 @@
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="11">
@@ -1965,7 +1965,7 @@
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11">
@@ -2033,7 +2033,7 @@
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="11">
@@ -2093,7 +2093,7 @@
     </row>
     <row r="21" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="11">
@@ -2162,7 +2162,7 @@
     </row>
     <row r="22" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="11">
@@ -2231,7 +2231,7 @@
     </row>
     <row r="23" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="11">
@@ -2300,7 +2300,7 @@
     </row>
     <row r="24" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11">
@@ -2369,7 +2369,7 @@
     </row>
     <row r="25" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11">
@@ -2438,7 +2438,7 @@
     </row>
     <row r="26" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11">
@@ -2507,7 +2507,7 @@
     </row>
     <row r="27" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="11">
@@ -2576,7 +2576,7 @@
     </row>
     <row r="28" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="11">
@@ -2645,7 +2645,7 @@
     </row>
     <row r="29" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="11">
@@ -2714,7 +2714,7 @@
     </row>
     <row r="30" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11">
@@ -2777,7 +2777,7 @@
     </row>
     <row r="31" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="11">
@@ -2838,7 +2838,7 @@
     </row>
     <row r="32" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="11">
@@ -2907,7 +2907,7 @@
     </row>
     <row r="33" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="11">
@@ -2976,7 +2976,7 @@
     </row>
     <row r="34" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="11">
@@ -3045,7 +3045,7 @@
     </row>
     <row r="35" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="11">
@@ -3114,7 +3114,7 @@
     </row>
     <row r="36" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="11">
@@ -3183,7 +3183,7 @@
     </row>
     <row r="37" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="11">
@@ -3252,7 +3252,7 @@
     </row>
     <row r="38" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="11">
@@ -3319,7 +3319,7 @@
     </row>
     <row r="39" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="11">
@@ -3386,7 +3386,7 @@
     </row>
     <row r="40" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="11">
@@ -3447,7 +3447,7 @@
     </row>
     <row r="41" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="11">
@@ -3516,7 +3516,7 @@
     </row>
     <row r="42" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" s="11"/>
       <c r="C42" s="11">
@@ -3585,7 +3585,7 @@
     </row>
     <row r="43" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="11">
@@ -3654,7 +3654,7 @@
     </row>
     <row r="44" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="11">
@@ -3723,7 +3723,7 @@
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="11"/>
       <c r="C45" s="11">
@@ -3791,7 +3791,7 @@
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="11">
@@ -3859,7 +3859,7 @@
     </row>
     <row r="47" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="11"/>
       <c r="C47" s="11">
@@ -3927,7 +3927,7 @@
     </row>
     <row r="48" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="11"/>
       <c r="C48" s="11">
@@ -3991,7 +3991,7 @@
     </row>
     <row r="49" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B49" s="11"/>
       <c r="C49" s="11">
@@ -4059,7 +4059,7 @@
     </row>
     <row r="50" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B50" s="11"/>
       <c r="C50" s="11">
@@ -4125,7 +4125,7 @@
     </row>
     <row r="51" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B51" s="11"/>
       <c r="C51" s="11">
@@ -4187,7 +4187,7 @@
     </row>
     <row r="52" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B52" s="11"/>
       <c r="C52" s="11">
@@ -4249,7 +4249,7 @@
     </row>
     <row r="53" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B53" s="11"/>
       <c r="C53" s="11">
@@ -4317,7 +4317,7 @@
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B54" s="11"/>
       <c r="C54" s="11">
@@ -4385,7 +4385,7 @@
     </row>
     <row r="55" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B55" s="11"/>
       <c r="C55" s="11">
@@ -4453,7 +4453,7 @@
     </row>
     <row r="56" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="11">
@@ -4521,7 +4521,7 @@
     </row>
     <row r="57" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B57" s="11"/>
       <c r="C57" s="11">
@@ -4589,7 +4589,7 @@
     </row>
     <row r="58" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B58" s="11"/>
       <c r="C58" s="11">
@@ -4657,7 +4657,7 @@
     </row>
     <row r="59" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B59" s="11"/>
       <c r="C59" s="11">
@@ -4725,7 +4725,7 @@
     </row>
     <row r="60" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B60" s="11"/>
       <c r="C60" s="11">
@@ -4821,34 +4821,34 @@
         <v>12</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>13</v>
@@ -4860,7 +4860,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
@@ -4909,7 +4909,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
@@ -4958,7 +4958,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -4978,7 +4978,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3">
@@ -5026,7 +5026,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
@@ -5074,7 +5074,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
@@ -5149,7 +5149,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>3</v>
@@ -5158,66 +5158,66 @@
         <v>10</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>96</v>
-      </c>
       <c r="M1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y1" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="S1" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2">
         <v>12.468036529680365</v>
@@ -5226,7 +5226,7 @@
         <v>44.2268326417704</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H2">
         <v>0.68</v>
@@ -5237,7 +5237,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <v>12.536529680365296</v>
@@ -5246,7 +5246,7 @@
         <v>44.253803596127248</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H3">
         <v>0.8</v>
@@ -5257,7 +5257,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4">
         <v>12.629756468797565</v>
@@ -5266,7 +5266,7 @@
         <v>44.289764868603044</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H4">
         <v>0.82</v>
@@ -5277,7 +5277,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5">
         <v>12.844748858447488</v>
@@ -5286,7 +5286,7 @@
         <v>44.374827109266946</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H5">
         <v>0.7</v>
@@ -5297,7 +5297,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6">
         <v>12.379566210045661</v>
@@ -5306,7 +5306,7 @@
         <v>44.742738589211619</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H6">
         <v>0.86</v>
@@ -5317,7 +5317,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7">
         <v>12.479452054794521</v>
@@ -5326,7 +5326,7 @@
         <v>44.744813278008301</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H7">
         <v>0.83</v>
@@ -5344,13 +5344,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -5376,7 +5376,7 @@
         <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -5384,7 +5384,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -5392,7 +5392,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -5400,7 +5400,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -5416,7 +5416,7 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -5424,7 +5424,7 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
@@ -5448,7 +5448,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
@@ -5464,17 +5464,17 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>